<commit_message>
se configuran vlan y se agregan servers funcionales
</commit_message>
<xml_diff>
--- a/Subneting FGE.xlsx
+++ b/Subneting FGE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elio Raymundo\Documents\UMG\SEMESTRE 9\Redes de computadoras II\Tareas y ejercicios\Proyecto final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elio Raymundo\Documents\UMG\SEMESTRE 9\Redes de computadoras II\Tareas y ejercicios\proyecto_final_redes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11616"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -188,10 +188,10 @@
     <t>Departamento de Direccion General</t>
   </si>
   <si>
-    <t>Departamento de Informática</t>
-  </si>
-  <si>
     <t>Departamento de Control de Gestión</t>
+  </si>
+  <si>
+    <t>Departamento de Informatica</t>
   </si>
 </sst>
 </file>
@@ -395,15 +395,6 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -429,13 +420,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,460 +719,461 @@
   <dimension ref="B1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="G22" sqref="C22:G22"/>
+      <selection activeCell="H24" sqref="H24:K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="5" width="18.28515625" customWidth="1"/>
+    <col min="4" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D2" s="1" t="s">
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" s="8">
         <v>128</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="9">
         <v>64</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="9">
         <v>32</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="9">
         <v>16</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="9">
         <v>8</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="9">
         <v>4</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="9">
         <v>2</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="9">
         <v>1</v>
       </c>
-      <c r="J10" s="12"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="13">
+      <c r="J10" s="9"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="10">
         <v>1</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="11">
         <v>1</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="11">
         <v>1</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="11">
         <v>0</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="11">
         <v>0</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="11">
         <v>0</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="11">
         <v>0</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="11">
         <v>0</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="12">
         <f xml:space="preserve"> 224</f>
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="10"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="7"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="21" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="F22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H22" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="4">
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C26" s="1">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="1">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="1">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H29" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="4">
-        <v>2</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="4">
-        <v>3</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="4">
-        <v>4</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="4">
-        <v>5</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="4">
-        <v>6</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="4">
-        <v>7</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H29" s="20" t="s">
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="1">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="4">
-        <v>8</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H30" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D2:I2"/>
     <mergeCell ref="H28:K28"/>
     <mergeCell ref="H29:K29"/>
     <mergeCell ref="H30:K30"/>
@@ -1182,7 +1183,6 @@
     <mergeCell ref="H25:K25"/>
     <mergeCell ref="H26:K26"/>
     <mergeCell ref="H27:K27"/>
-    <mergeCell ref="D2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>